<commit_message>
docs: use case description 수정
</commit_message>
<xml_diff>
--- a/usecase_description_강지완.xlsx
+++ b/usecase_description_강지완.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lecture\24-1\소프트웨어공학\팀플\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SE_Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0348730-D7CA-4B1A-B3D3-31D7B917ABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591CC6AC-F9FD-4D56-B3FC-F62ED6AF8645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,10 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3. 로그인 페이지 또는 홈 화면으로 리디렉션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 관리자가 대여소 등록 메뉴 선택</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -114,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7. 저장된 대여소 정보 화면을 표시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>자전거 대여소 리스트 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -151,6 +143,30 @@
   </si>
   <si>
     <t>8. 시스템은 해당 대여소를 DB에서 삭제하고 리스트를 갱신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use Case Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. 시스템은 삭제 확인 메시지를 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 시스템은 저장된 대여소 정보 화면을 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 시스템은 로그아웃 완료 메시지 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 로그인 페이지 또는 홈 화면으로 리디렉션</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,8 +191,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -192,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -222,35 +246,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -264,6 +260,41 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -275,32 +306,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -309,17 +328,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,226 +707,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32EF711-E41E-4776-BBB7-C6C14271EF27}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="60.625" customWidth="1"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="60.625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="60.625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="49.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="49.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
+    <row r="29" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-    </row>
-    <row r="25" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="49.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3" t="s">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="33" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3" t="s">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="35" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3" t="s">
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3" t="s">
-        <v>28</v>
+    <row r="37" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A25:B25"/>
+  <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>